<commit_message>
Added charts at constant 2017 prices
</commit_message>
<xml_diff>
--- a/GDP.xlsx
+++ b/GDP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="macro_economic" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
     <sheet name="expenditure_cp" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="expenditure_c2017" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="expenditure_deflator" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="TABLE2" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="constant_2017" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="TABLE2AA" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="TABLE2B" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="TABLE3" sheetId="13" state="visible" r:id="rId14"/>
@@ -3232,8 +3232,8 @@
   </sheetPr>
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3243,7 +3243,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>38</v>
@@ -32905,7 +32905,7 @@
   </sheetPr>
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected GDP Summary Bugs
</commit_message>
<xml_diff>
--- a/GDP.xlsx
+++ b/GDP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="macro_economic" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="95">
   <si>
     <t xml:space="preserve">Years</t>
   </si>
@@ -301,16 +301,22 @@
     <t xml:space="preserve">        Import Services</t>
   </si>
   <si>
-    <t xml:space="preserve">        Goods (fob)</t>
+    <t xml:space="preserve">         Import Services</t>
   </si>
   <si>
-    <t xml:space="preserve">         Services</t>
+    <t xml:space="preserve">       Export Goods (fob)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Export Services</t>
   </si>
   <si>
     <t xml:space="preserve">        Import Goods (fob)</t>
   </si>
   <si>
-    <t xml:space="preserve">         Import Services</t>
+    <t xml:space="preserve">        Goods (fob)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Services</t>
   </si>
 </sst>
 </file>
@@ -3318,8 +3324,8 @@
   </sheetPr>
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3362,19 +3368,19 @@
         <v>83</v>
       </c>
       <c r="M1" s="64" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N1" s="64" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O1" s="65" t="s">
         <v>86</v>
       </c>
       <c r="P1" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q1" s="66" t="s">
         <v>89</v>
-      </c>
-      <c r="Q1" s="66" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4667,8 +4673,8 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4708,19 +4714,19 @@
         <v>83</v>
       </c>
       <c r="L1" s="64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M1" s="64" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N1" s="65" t="s">
         <v>86</v>
       </c>
       <c r="O1" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="66" t="s">
         <v>89</v>
-      </c>
-      <c r="P1" s="66" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,10 +6004,10 @@
         <v>86</v>
       </c>
       <c r="P1" s="75" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q1" s="76" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7335,19 +7341,19 @@
         <v>83</v>
       </c>
       <c r="K1" s="83" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="L1" s="83" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M1" s="83" t="s">
         <v>86</v>
       </c>
       <c r="N1" s="83" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="O1" s="84" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" s="87" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>